<commit_message>
Script is working till company creating
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\git\MainShare\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bacancy\eclipse-workspace\ShareDataDrivenFramwork\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84C2B90-DA6A-4C5A-A1FF-288E4189711A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="test_suite" sheetId="3" r:id="rId1"/>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="GitHubSync" sheetId="4" r:id="rId3"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>FirstName</t>
   </si>
@@ -96,12 +96,24 @@
   </si>
   <si>
     <t>GitHubSync</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>companyname</t>
+  </si>
+  <si>
+    <t>vase123</t>
+  </si>
+  <si>
+    <t>bhautik-vase45</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -412,16 +424,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -429,7 +441,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -444,16 +456,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +482,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -487,7 +499,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -504,7 +516,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -521,7 +533,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -545,16 +557,47 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -562,7 +605,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
create account is completed
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>FirstName</t>
   </si>
@@ -104,10 +104,16 @@
     <t>companyname</t>
   </si>
   <si>
-    <t>vase123</t>
-  </si>
-  <si>
-    <t>bhautik-vase45</t>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>FREE</t>
+  </si>
+  <si>
+    <t>bhautik-vasebh</t>
+  </si>
+  <si>
+    <t>bh</t>
   </si>
 </sst>
 </file>
@@ -558,32 +564,43 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
GitHub Sync done (#12)
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata.xlsx
+++ b/src/test/resources/excel/testdata.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>FirstName</t>
   </si>
@@ -110,10 +110,16 @@
     <t>FREE</t>
   </si>
   <si>
-    <t>bhautik-vasebh</t>
-  </si>
-  <si>
     <t>bh</t>
+  </si>
+  <si>
+    <t>orgURL</t>
+  </si>
+  <si>
+    <t>https://github.com/orgs/dineflesh</t>
+  </si>
+  <si>
+    <t>bhautik-vasebh1</t>
   </si>
 </sst>
 </file>
@@ -564,10 +570,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,7 +582,7 @@
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -586,16 +592,22 @@
       <c r="C1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>28</v>
       </c>
       <c r="C2" t="s">
         <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>